<commit_message>
remove index for title
</commit_message>
<xml_diff>
--- a/audible/bestSellers.xlsx
+++ b/audible/bestSellers.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1. The Let Them Theory</t>
+          <t>The Let Them Theory</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -480,7 +480,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2. Quicksilver</t>
+          <t>Quicksilver</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -502,7 +502,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3. Defiance of the Fall 14</t>
+          <t>Defiance of the Fall 14</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -517,14 +517,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">6 </t>
+          <t xml:space="preserve">7 </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4. How My Neighbor Stole Christmas</t>
+          <t>How My Neighbor Stole Christmas</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -546,7 +546,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5. The Boyfriend</t>
+          <t>The Boyfriend</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6. Fourth Wing</t>
+          <t>Fourth Wing</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -590,7 +590,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7. Onyx Storm</t>
+          <t>Onyx Storm</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -612,7 +612,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8. The Housemaid</t>
+          <t>The Housemaid</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9. Iron Flame</t>
+          <t>Iron Flame</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -649,14 +649,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">28,308 </t>
+          <t xml:space="preserve">28,309 </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10. 48 Laws of Power</t>
+          <t>48 Laws of Power</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -678,7 +678,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11. Fourth Wing (Part 1 of 2) (Dramatized Adaptation)</t>
+          <t>Fourth Wing (Part 1 of 2) (Dramatized Adaptation)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12. A Court of Mist and Fury</t>
+          <t>A Court of Mist and Fury</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -722,7 +722,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>13. Fourth Wing (Part 2 of 2) (Dramatized Adaptation)</t>
+          <t>Fourth Wing (Part 2 of 2) (Dramatized Adaptation)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -744,7 +744,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>14. Cher: Part One</t>
+          <t>Cher: Part One</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -766,7 +766,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>15. Madness</t>
+          <t>Madness</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16. A Court of Wings and Ruin</t>
+          <t>A Court of Wings and Ruin</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -803,14 +803,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">38,344 </t>
+          <t xml:space="preserve">38,345 </t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17. The Housemaid Is Watching</t>
+          <t>The Housemaid Is Watching</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18. Beware of Chicken 4: A Xianxia Cultivation Novel</t>
+          <t>Beware of Chicken 4: A Xianxia Cultivation Novel</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -854,7 +854,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19. Project Hail Mary</t>
+          <t>Project Hail Mary</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -869,14 +869,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">183,327 </t>
+          <t xml:space="preserve">183,328 </t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20. Knight of Shadows</t>
+          <t>Knight of Shadows</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -898,7 +898,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>21. It Ends with Us</t>
+          <t>It Ends with Us</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -920,7 +920,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>22. Iron Flame (Part 1 of 2) (Dramatized Adaptation)</t>
+          <t>Iron Flame (Part 1 of 2) (Dramatized Adaptation)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -942,7 +942,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>23. The Most Wonderful Crime of the Year</t>
+          <t>The Most Wonderful Crime of the Year</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>24. The Psychology of Money</t>
+          <t>The Psychology of Money</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -986,7 +986,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>25. The Locked Door</t>
+          <t>The Locked Door</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>26. The Housemaid's Secret</t>
+          <t>The Housemaid's Secret</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1030,7 +1030,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>27. The Subtle Art of Not Giving a F*ck</t>
+          <t>The Subtle Art of Not Giving a F*ck</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1052,7 +1052,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>28. Queen of Shadows</t>
+          <t>Queen of Shadows</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1074,7 +1074,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>29. Iron Flame (Part 2 of 2) (Dramatized Adaptation)</t>
+          <t>Iron Flame (Part 2 of 2) (Dramatized Adaptation)</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1096,7 +1096,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>30. Mark of the Fool 7</t>
+          <t>Mark of the Fool 7</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1111,14 +1111,14 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve">585 </t>
+          <t xml:space="preserve">588 </t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>31. A Court of Silver Flames</t>
+          <t>A Court of Silver Flames</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1140,7 +1140,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>32. Don't Believe Everything You Think (Expanded Edition)</t>
+          <t>Don't Believe Everything You Think (Expanded Edition)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1162,7 +1162,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>33. Butcher &amp; Blackbird</t>
+          <t>Butcher &amp; Blackbird</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1184,7 +1184,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>34. Verity</t>
+          <t>Verity</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1206,7 +1206,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>35. Kingdom of Ash</t>
+          <t>Kingdom of Ash</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>36. Empire of Storms</t>
+          <t>Empire of Storms</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1250,7 +1250,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>37. Tower of Dawn</t>
+          <t>Tower of Dawn</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1272,7 +1272,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>38. That's Not My Name</t>
+          <t>That's Not My Name</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1294,7 +1294,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>39. The Mountain Is You</t>
+          <t>The Mountain Is You</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1316,7 +1316,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>40. How to Talk to Anyone</t>
+          <t>How to Talk to Anyone</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1338,7 +1338,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>41. Can't Hurt Me</t>
+          <t>Can't Hurt Me</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1360,7 +1360,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>42. Dungeon Crawler Carl</t>
+          <t>Dungeon Crawler Carl</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1382,7 +1382,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>43. My Favorite Holidate</t>
+          <t>My Favorite Holidate</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1404,7 +1404,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>44. My Time to Stand</t>
+          <t>My Time to Stand</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1426,7 +1426,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>45. How to Win Friends &amp; Influence People</t>
+          <t>How to Win Friends &amp; Influence People</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>46. Dune</t>
+          <t>Dune</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1470,7 +1470,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>47. Never Lie</t>
+          <t>Never Lie</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>48. Haunting Adeline</t>
+          <t>Haunting Adeline</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1514,7 +1514,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>49. A Court of Mist and Fury (Part 1 of 2) (Dramatized Adaptation)</t>
+          <t>A Court of Mist and Fury (Part 1 of 2) (Dramatized Adaptation)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1536,7 +1536,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>50. The Ritual</t>
+          <t>The Ritual</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1558,7 +1558,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>51. Phantasma</t>
+          <t>Phantasma</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1580,7 +1580,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>52. The Teacher</t>
+          <t>The Teacher</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1602,7 +1602,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>53. The Chronicles of Narnia Complete Audio Collection</t>
+          <t>The Chronicles of Narnia Complete Audio Collection</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1624,7 +1624,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>54. Remarkably Bright Creatures</t>
+          <t>Remarkably Bright Creatures</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1646,7 +1646,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>55. The Serpent and the Wings of Night</t>
+          <t>The Serpent and the Wings of Night</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>56. The Four Agreements</t>
+          <t>The Four Agreements</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1690,7 +1690,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>57. Outlive</t>
+          <t>Outlive</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1712,7 +1712,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>58. Rich Dad Poor Dad: 20th Anniversary Edition</t>
+          <t>Rich Dad Poor Dad: 20th Anniversary Edition</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1734,7 +1734,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>59. Unfu*k Yourself</t>
+          <t>Unfu*k Yourself</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1756,7 +1756,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>60. The Ashes and the Star-Cursed King</t>
+          <t>The Ashes and the Star-Cursed King</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>61. Not Till We Are Lost</t>
+          <t>Not Till We Are Lost</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1800,7 +1800,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>62. The Legend of Randidly Ghosthound 8</t>
+          <t>The Legend of Randidly Ghosthound 8</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1822,7 +1822,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>63. The Briar Club</t>
+          <t>The Briar Club</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1844,7 +1844,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>64. The Art of Letting Go: Stop Overthinking, Stop Negative Spirals, and Find Emotional Freedom</t>
+          <t>The Art of Letting Go: Stop Overthinking, Stop Negative Spirals, and Find Emotional Freedom</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1866,7 +1866,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>65. House of Flame and Shadow (Part 1 of 2) (Dramatized Adaptation)</t>
+          <t>House of Flame and Shadow (Part 1 of 2) (Dramatized Adaptation)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1888,7 +1888,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>66. Man's Search for Meaning</t>
+          <t>Man's Search for Meaning</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1910,7 +1910,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>67. A Court of Wings and Ruin (1 of 3) [Dramatized Adaptation]</t>
+          <t>A Court of Wings and Ruin (1 of 3) [Dramatized Adaptation]</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1932,7 +1932,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>68. Extreme Ownership</t>
+          <t>Extreme Ownership</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1954,7 +1954,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>69. Adult Children of Emotionally Immature Parents</t>
+          <t>Adult Children of Emotionally Immature Parents</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1976,7 +1976,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>70. The Power of Now</t>
+          <t>The Power of Now</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1998,7 +1998,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>71. Does It Hurt?</t>
+          <t>Does It Hurt?</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2020,7 +2020,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>72. Variation</t>
+          <t>Variation</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2042,7 +2042,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>73. Spark of the Everflame</t>
+          <t>Spark of the Everflame</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2064,7 +2064,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>74. Carl's Doomsday Scenario</t>
+          <t>Carl's Doomsday Scenario</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2086,7 +2086,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>75. A Court of Mist and Fury (Part 2 of 2) (Dramatized Adaptation)</t>
+          <t>A Court of Mist and Fury (Part 2 of 2) (Dramatized Adaptation)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>76. When the Moon Hatched</t>
+          <t>When the Moon Hatched</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2130,7 +2130,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>77. The Plight Before Christmas</t>
+          <t>The Plight Before Christmas</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2152,7 +2152,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>78. Hunting Adeline</t>
+          <t>Hunting Adeline</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2174,7 +2174,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>79. Glow of the Everflame</t>
+          <t>Glow of the Everflame</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2196,7 +2196,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>80. Hillbilly Elegy</t>
+          <t>Hillbilly Elegy</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2218,7 +2218,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>81. The Christmas Fix</t>
+          <t>The Christmas Fix</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2240,7 +2240,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>82. Demon Copperhead</t>
+          <t>Demon Copperhead</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2262,7 +2262,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>83. Cozy Witch Mysteries: Special Edition Box Set of 8 Books</t>
+          <t>Cozy Witch Mysteries: Special Edition Box Set of 8 Books</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2284,7 +2284,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>84. The 7 Habits of Highly Effective People</t>
+          <t>The 7 Habits of Highly Effective People</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2306,7 +2306,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>85. I Want to Trust You, but I Don't</t>
+          <t>I Want to Trust You, but I Don't</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2328,7 +2328,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>86. The Christmas Bookshop</t>
+          <t>The Christmas Bookshop</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2350,7 +2350,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>87. This Inevitable Ruin</t>
+          <t>This Inevitable Ruin</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2372,7 +2372,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>88. The Dungeon Anarchist's Cookbook</t>
+          <t>The Dungeon Anarchist's Cookbook</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2394,7 +2394,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>89. The Songbird and the Heart of Stone</t>
+          <t>The Songbird and the Heart of Stone</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2416,7 +2416,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>90. Credence</t>
+          <t>Credence</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>91. I'm Glad My Mom Died</t>
+          <t>I'm Glad My Mom Died</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2460,7 +2460,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>92. The Gate of the Feral Gods</t>
+          <t>The Gate of the Feral Gods</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2482,7 +2482,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>93. I Will Teach You to Be Rich</t>
+          <t>I Will Teach You to Be Rich</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2504,7 +2504,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>94. The Silmarillion</t>
+          <t>The Silmarillion</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2526,7 +2526,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>95. A Kingdom of Flesh and Fire</t>
+          <t>A Kingdom of Flesh and Fire</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2548,7 +2548,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>96. The Inmate</t>
+          <t>The Inmate</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2570,7 +2570,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>97. Hábitos atómicos (Español neutro)</t>
+          <t>Hábitos atómicos (Español neutro)</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2592,7 +2592,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>98. Flock</t>
+          <t>Flock</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2614,7 +2614,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>99. Think This, Not That</t>
+          <t>Think This, Not That</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2636,7 +2636,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>100. Think and Grow Rich</t>
+          <t>Think and Grow Rich</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">

</xml_diff>